<commit_message>
add list staff schedule
</commit_message>
<xml_diff>
--- a/src/models/data/schedule.xlsx
+++ b/src/models/data/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dhieu\Learn\Hoc_Ki_VIII\src\MEDRE_BE\src\models\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C16E18-A20A-40A4-ACD9-1DBCE3A5F73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3291FC4-2274-41ED-9CDA-7579BCD309DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3168" yWindow="2184" windowWidth="19224" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="19224" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="70">
   <si>
     <t>id</t>
   </si>
@@ -210,6 +210,42 @@
   </si>
   <si>
     <t>4600b1d8-e1bf-41a9-9ff9-2a64ad2a194a</t>
+  </si>
+  <si>
+    <t>2023-03-30</t>
+  </si>
+  <si>
+    <t>2023-03-31</t>
+  </si>
+  <si>
+    <t>2023-04-01</t>
+  </si>
+  <si>
+    <t>2023-04-02</t>
+  </si>
+  <si>
+    <t>2023-04-03</t>
+  </si>
+  <si>
+    <t>2023-04-04</t>
+  </si>
+  <si>
+    <t>2023-04-05</t>
+  </si>
+  <si>
+    <t>2023-04-06</t>
+  </si>
+  <si>
+    <t>2023-04-07</t>
+  </si>
+  <si>
+    <t>2023-04-08</t>
+  </si>
+  <si>
+    <t>2023-04-09</t>
+  </si>
+  <si>
+    <t>2023-04-10</t>
   </si>
 </sst>
 </file>
@@ -259,7 +295,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:G67"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +588,7 @@
     <col min="1" max="1" width="36.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.21875" customWidth="1"/>
     <col min="3" max="3" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="58.6640625" bestFit="1" customWidth="1"/>
@@ -572,7 +608,7 @@
       <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E1" t="s">
@@ -592,8 +628,8 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
-        <v>45015</v>
+      <c r="D2" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
@@ -612,8 +648,8 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
-        <v>45016</v>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>42</v>
@@ -632,8 +668,8 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
-        <v>45017</v>
+      <c r="D4" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="E4" t="s">
         <v>38</v>
@@ -652,8 +688,8 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
-        <v>45018</v>
+      <c r="D5" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="E5" t="s">
         <v>38</v>
@@ -672,8 +708,8 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
-        <v>45019</v>
+      <c r="D6" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="E6" t="s">
         <v>42</v>
@@ -692,8 +728,8 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1">
-        <v>45020</v>
+      <c r="D7" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E7" t="s">
         <v>38</v>
@@ -712,8 +748,8 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1">
-        <v>45021</v>
+      <c r="D8" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="E8" t="s">
         <v>42</v>
@@ -732,8 +768,8 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1">
-        <v>45022</v>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
@@ -752,8 +788,8 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1">
-        <v>45023</v>
+      <c r="D10" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
@@ -772,8 +808,8 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1">
-        <v>45015</v>
+      <c r="D11" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E11" t="s">
         <v>38</v>
@@ -792,8 +828,8 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="1">
-        <v>45016</v>
+      <c r="D12" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="E12" t="s">
         <v>38</v>
@@ -812,8 +848,8 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1">
-        <v>45017</v>
+      <c r="D13" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>
@@ -832,8 +868,8 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="1">
-        <v>45018</v>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
@@ -852,8 +888,8 @@
       <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1">
-        <v>45019</v>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="E15" t="s">
         <v>38</v>
@@ -872,8 +908,8 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1">
-        <v>45020</v>
+      <c r="D16" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E16" t="s">
         <v>38</v>
@@ -892,8 +928,8 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="1">
-        <v>45021</v>
+      <c r="D17" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="E17" t="s">
         <v>38</v>
@@ -912,8 +948,8 @@
       <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="1">
-        <v>45019</v>
+      <c r="D18" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="E18" t="s">
         <v>38</v>
@@ -932,8 +968,8 @@
       <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="1">
-        <v>45020</v>
+      <c r="D19" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E19" t="s">
         <v>38</v>
@@ -952,8 +988,8 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="1">
-        <v>45021</v>
+      <c r="D20" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="E20" t="s">
         <v>38</v>
@@ -972,8 +1008,8 @@
       <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1">
-        <v>45019</v>
+      <c r="D21" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E21" t="s">
         <v>42</v>
@@ -992,8 +1028,8 @@
       <c r="C22" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
-        <v>45020</v>
+      <c r="D22" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="E22" t="s">
         <v>38</v>
@@ -1012,8 +1048,8 @@
       <c r="C23" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="1">
-        <v>45021</v>
+      <c r="D23" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="E23" t="s">
         <v>42</v>
@@ -1032,8 +1068,8 @@
       <c r="C24" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="1">
-        <v>45021</v>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="E24" t="s">
         <v>38</v>
@@ -1052,8 +1088,8 @@
       <c r="C25" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="1">
-        <v>45019</v>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E25" t="s">
         <v>38</v>
@@ -1072,8 +1108,8 @@
       <c r="C26" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="1">
-        <v>45020</v>
+      <c r="D26" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="E26" t="s">
         <v>38</v>
@@ -1092,8 +1128,8 @@
       <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="1">
-        <v>45017</v>
+      <c r="D27" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="E27" t="s">
         <v>42</v>
@@ -1112,8 +1148,8 @@
       <c r="C28" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="1">
-        <v>45018</v>
+      <c r="D28" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="E28" t="s">
         <v>38</v>
@@ -1132,8 +1168,8 @@
       <c r="C29" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="1">
-        <v>45019</v>
+      <c r="D29" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="E29" t="s">
         <v>38</v>

</xml_diff>